<commit_message>
update the excel click URL file
</commit_message>
<xml_diff>
--- a/Click URLs.xlsx
+++ b/Click URLs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\RPA_OCR_Extraction_Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C79B798-A1C9-45C1-A8F5-991598CA255A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5560A8-77E7-4755-A5D8-DF54EA5095B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="-14415" windowWidth="24675" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Value</t>
   </si>
@@ -97,6 +97,105 @@
   </si>
   <si>
     <t>Online Disability Appeal Application (&amp;quot;iAppeal&amp;quot;)</t>
+  </si>
+  <si>
+    <t>Folder Path</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-827\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-1696\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-8000\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"Fillable SSA-8000\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-8001\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-3369\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-821\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"HA-1151\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"HA-1152\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-787\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-1699\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"paper form\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-3373\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-3820\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-3375\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"3376\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"3377\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"3378\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"3379\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-5665\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"Compassionate Allowances\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"SSA-4814\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"Listing of Impairments\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"Online Disability Appeal Application\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56"+"\"+"Medicaid Eligibility Income\"</t>
+  </si>
+  <si>
+    <t>"Website ID 56+"\"+"SSA-3288\"</t>
+  </si>
+  <si>
+    <t>Folder Path 2</t>
+  </si>
+  <si>
+    <t>Website ID 56+\+SSA-3288\</t>
+  </si>
+  <si>
+    <t>Website ID 56+\+SSA-827\</t>
+  </si>
+  <si>
+    <t>Website ID 56+\+SSA-1696\</t>
+  </si>
+  <si>
+    <t>Website ID 56+\+SSA-8000\</t>
+  </si>
+  <si>
+    <t>Website ID 56+\+Fillable SSA-8000\</t>
   </si>
 </sst>
 </file>
@@ -445,160 +544,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="57.21875" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>3376</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>3377</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>3378</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>3379</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new click activity and modified the selector
</commit_message>
<xml_diff>
--- a/Click URLs.xlsx
+++ b/Click URLs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\RPA_OCR_Extraction_Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5560A8-77E7-4755-A5D8-DF54EA5095B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C8630B-9DCB-4602-9543-C81EF4E91E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="-14415" windowWidth="24675" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>